<commit_message>
edit dan delete ahli
</commit_message>
<xml_diff>
--- a/database/tb_ahli.xlsx
+++ b/database/tb_ahli.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,69 +463,58 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P3</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="n">
-        <v>20</v>
-      </c>
-      <c r="C5" t="n">
-        <v>20</v>
-      </c>
-      <c r="D5" t="n">
-        <v>20</v>
-      </c>
-      <c r="E5" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix hapus and username
</commit_message>
<xml_diff>
--- a/database/tb_ahli.xlsx
+++ b/database/tb_ahli.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,80 +458,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P3</t>
         </is>
       </c>
       <c r="B2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
         <v>8</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P3</t>
+          <t>P6</t>
         </is>
       </c>
       <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
         <v>9</v>
       </c>
-      <c r="C3" t="n">
-        <v>3</v>
-      </c>
       <c r="D3" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>P4</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>10</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>P5</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="C5" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>P6</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>7</v>
-      </c>
-      <c r="C6" t="n">
-        <v>9</v>
-      </c>
-      <c r="D6" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>